<commit_message>
Agregamos la teoria de conjuntos entre 2 entidades
</commit_message>
<xml_diff>
--- a/trabajo del minimarket.xlsx
+++ b/trabajo del minimarket.xlsx
@@ -5,18 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bases de datos CECEP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zarkp\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D6F406-126A-420F-9120-28A30CA73780}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72987DB6-DBBB-483F-9AD0-2A00FD6B7D72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Levantamiento" sheetId="1" r:id="rId1"/>
     <sheet name="Entidades" sheetId="2" r:id="rId2"/>
     <sheet name="Estructura" sheetId="3" r:id="rId3"/>
     <sheet name="Relaciones" sheetId="4" r:id="rId4"/>
+    <sheet name="P U D" sheetId="5" r:id="rId5"/>
+    <sheet name="E U C" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="143">
   <si>
     <t>Entidades Fuertes</t>
   </si>
@@ -414,6 +416,60 @@
   </si>
   <si>
     <t>Refresco en Pol.</t>
+  </si>
+  <si>
+    <t>Productos==&gt;P</t>
+  </si>
+  <si>
+    <t>D&lt;==Detalle</t>
+  </si>
+  <si>
+    <t>P.Id_producto</t>
+  </si>
+  <si>
+    <t>D.Id_producto</t>
+  </si>
+  <si>
+    <t>D.Total_prod</t>
+  </si>
+  <si>
+    <t>P.Marca</t>
+  </si>
+  <si>
+    <t>P.Precio</t>
+  </si>
+  <si>
+    <t>Consulta</t>
+  </si>
+  <si>
+    <t>P U D</t>
+  </si>
+  <si>
+    <t>P U D=[X/X   E C v XEE</t>
+  </si>
+  <si>
+    <t>E U C</t>
+  </si>
+  <si>
+    <t>E.Id_empleado</t>
+  </si>
+  <si>
+    <t>C.Num_caja</t>
+  </si>
+  <si>
+    <t>E.Fecha</t>
+  </si>
+  <si>
+    <t>E.Nom_empleado</t>
+  </si>
+  <si>
+    <t>E.Turno</t>
+  </si>
+  <si>
+    <t>Empleado ==&gt;</t>
+  </si>
+  <si>
+    <t>&lt;==Caja</t>
   </si>
 </sst>
 </file>
@@ -425,7 +481,7 @@
     <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="166" formatCode="&quot;$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -469,6 +525,21 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="17">
@@ -569,7 +640,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -666,11 +737,100 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -783,10 +943,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="1" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="1" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="1" fillId="16" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="1" fillId="16" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -859,6 +1039,38 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="16" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2439,24 +2651,24 @@
   <sheetData>
     <row r="1" spans="1:8" ht="14.25" customHeight="1"/>
     <row r="2" spans="1:8" ht="14.25" customHeight="1">
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="52"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="61"/>
+      <c r="E2" s="61"/>
+      <c r="F2" s="61"/>
+      <c r="G2" s="61"/>
+      <c r="H2" s="62"/>
     </row>
     <row r="3" spans="1:8" ht="14.25" customHeight="1">
       <c r="B3" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="53" t="s">
+      <c r="C3" s="63" t="s">
         <v>71</v>
       </c>
-      <c r="D3" s="52"/>
+      <c r="D3" s="62"/>
       <c r="E3" s="25" t="s">
         <v>72</v>
       </c>
@@ -2473,15 +2685,15 @@
     <row r="4" spans="1:8" ht="14.25" customHeight="1"/>
     <row r="5" spans="1:8" ht="14.25" customHeight="1"/>
     <row r="6" spans="1:8" ht="14.25" customHeight="1">
-      <c r="B6" s="54" t="s">
+      <c r="B6" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="52"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="61"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="62"/>
     </row>
     <row r="7" spans="1:8" ht="14.25" customHeight="1">
       <c r="B7" s="24" t="s">
@@ -2493,32 +2705,32 @@
       <c r="D7" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="55" t="s">
+      <c r="E7" s="65" t="s">
         <v>51</v>
       </c>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="52"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="62"/>
     </row>
     <row r="8" spans="1:8" ht="14.25" customHeight="1">
       <c r="B8" s="28"/>
       <c r="C8" s="28"/>
       <c r="D8" s="28"/>
-      <c r="E8" s="56"/>
-      <c r="F8" s="57"/>
-      <c r="G8" s="57"/>
+      <c r="E8" s="66"/>
+      <c r="F8" s="67"/>
+      <c r="G8" s="67"/>
     </row>
     <row r="9" spans="1:8" ht="14.25" customHeight="1"/>
     <row r="10" spans="1:8" ht="14.25" customHeight="1">
-      <c r="B10" s="58" t="s">
+      <c r="B10" s="68" t="s">
         <v>75</v>
       </c>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="51"/>
-      <c r="H10" s="52"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="61"/>
+      <c r="H10" s="62"/>
     </row>
     <row r="11" spans="1:8" ht="14.25" customHeight="1">
       <c r="B11" s="24" t="s">
@@ -2533,35 +2745,35 @@
       <c r="E11" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="F11" s="53" t="s">
+      <c r="F11" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="G11" s="51"/>
-      <c r="H11" s="52"/>
+      <c r="G11" s="61"/>
+      <c r="H11" s="62"/>
     </row>
     <row r="12" spans="1:8" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:8" ht="14.25" customHeight="1"/>
     <row r="14" spans="1:8" ht="14.25" customHeight="1">
-      <c r="B14" s="63" t="s">
+      <c r="B14" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="52"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="61"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="61"/>
+      <c r="H14" s="62"/>
     </row>
     <row r="15" spans="1:8" ht="14.25" customHeight="1">
-      <c r="B15" s="64" t="s">
+      <c r="B15" s="74" t="s">
         <v>77</v>
       </c>
-      <c r="C15" s="51"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="52"/>
+      <c r="C15" s="61"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="61"/>
+      <c r="G15" s="61"/>
+      <c r="H15" s="62"/>
     </row>
     <row r="16" spans="1:8" ht="14.25" customHeight="1">
       <c r="A16" s="28"/>
@@ -2574,15 +2786,15 @@
     </row>
     <row r="17" spans="2:10" ht="14.25" customHeight="1"/>
     <row r="18" spans="2:10" ht="14.25" customHeight="1">
-      <c r="B18" s="65" t="s">
+      <c r="B18" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="C18" s="51"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="51"/>
-      <c r="G18" s="51"/>
-      <c r="H18" s="52"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="61"/>
+      <c r="F18" s="61"/>
+      <c r="G18" s="61"/>
+      <c r="H18" s="62"/>
     </row>
     <row r="19" spans="2:10" ht="14.25" customHeight="1">
       <c r="B19" s="24" t="s">
@@ -2600,51 +2812,51 @@
       <c r="F19" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="G19" s="55" t="s">
+      <c r="G19" s="65" t="s">
         <v>80</v>
       </c>
-      <c r="H19" s="52"/>
+      <c r="H19" s="62"/>
     </row>
     <row r="20" spans="2:10" ht="14.25" customHeight="1"/>
     <row r="21" spans="2:10" ht="14.25" customHeight="1"/>
     <row r="22" spans="2:10" ht="14.25" customHeight="1">
-      <c r="B22" s="66" t="s">
+      <c r="B22" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="51"/>
-      <c r="D22" s="51"/>
-      <c r="E22" s="51"/>
-      <c r="F22" s="51"/>
-      <c r="G22" s="51"/>
-      <c r="H22" s="52"/>
+      <c r="C22" s="61"/>
+      <c r="D22" s="61"/>
+      <c r="E22" s="61"/>
+      <c r="F22" s="61"/>
+      <c r="G22" s="61"/>
+      <c r="H22" s="62"/>
     </row>
     <row r="23" spans="2:10" ht="14.25" customHeight="1">
-      <c r="B23" s="67" t="s">
+      <c r="B23" s="77" t="s">
         <v>78</v>
       </c>
-      <c r="C23" s="52"/>
+      <c r="C23" s="62"/>
       <c r="D23" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="E23" s="55" t="s">
+      <c r="E23" s="65" t="s">
         <v>55</v>
       </c>
-      <c r="F23" s="51"/>
-      <c r="G23" s="51"/>
-      <c r="H23" s="52"/>
+      <c r="F23" s="61"/>
+      <c r="G23" s="61"/>
+      <c r="H23" s="62"/>
     </row>
     <row r="24" spans="2:10" ht="14.25" customHeight="1"/>
     <row r="25" spans="2:10" ht="14.25" customHeight="1"/>
     <row r="26" spans="2:10" ht="14.25" customHeight="1">
-      <c r="B26" s="59" t="s">
+      <c r="B26" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="51"/>
-      <c r="D26" s="51"/>
-      <c r="E26" s="51"/>
-      <c r="F26" s="51"/>
-      <c r="G26" s="51"/>
-      <c r="H26" s="52"/>
+      <c r="C26" s="61"/>
+      <c r="D26" s="61"/>
+      <c r="E26" s="61"/>
+      <c r="F26" s="61"/>
+      <c r="G26" s="61"/>
+      <c r="H26" s="62"/>
     </row>
     <row r="27" spans="2:10" ht="14.25" customHeight="1">
       <c r="B27" s="24" t="s">
@@ -2656,42 +2868,42 @@
       <c r="D27" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="E27" s="55" t="s">
+      <c r="E27" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="F27" s="51"/>
-      <c r="G27" s="51"/>
-      <c r="H27" s="52"/>
+      <c r="F27" s="61"/>
+      <c r="G27" s="61"/>
+      <c r="H27" s="62"/>
     </row>
     <row r="28" spans="2:10" ht="14.25" customHeight="1"/>
     <row r="29" spans="2:10" ht="14.25" customHeight="1"/>
     <row r="30" spans="2:10" ht="14.25" customHeight="1">
-      <c r="B30" s="60" t="s">
+      <c r="B30" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="51"/>
-      <c r="D30" s="51"/>
-      <c r="E30" s="51"/>
-      <c r="F30" s="51"/>
-      <c r="G30" s="51"/>
-      <c r="H30" s="52"/>
+      <c r="C30" s="61"/>
+      <c r="D30" s="61"/>
+      <c r="E30" s="61"/>
+      <c r="F30" s="61"/>
+      <c r="G30" s="61"/>
+      <c r="H30" s="62"/>
     </row>
     <row r="31" spans="2:10" ht="14.25" customHeight="1">
-      <c r="B31" s="61" t="s">
+      <c r="B31" s="71" t="s">
         <v>81</v>
       </c>
-      <c r="C31" s="52"/>
+      <c r="C31" s="62"/>
       <c r="D31" s="27" t="s">
         <v>19</v>
       </c>
       <c r="E31" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="F31" s="62" t="s">
+      <c r="F31" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="G31" s="51"/>
-      <c r="H31" s="52"/>
+      <c r="G31" s="61"/>
+      <c r="H31" s="62"/>
     </row>
     <row r="32" spans="2:10" ht="14.25" customHeight="1">
       <c r="I32" s="31"/>
@@ -3716,38 +3928,38 @@
     <row r="2" spans="2:28" ht="14.25" customHeight="1"/>
     <row r="3" spans="2:28" ht="14.25" customHeight="1"/>
     <row r="4" spans="2:28" ht="14.25" customHeight="1">
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="52"/>
-      <c r="I4" s="65" t="s">
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="62"/>
+      <c r="I4" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="J4" s="51"/>
-      <c r="K4" s="51"/>
-      <c r="L4" s="51"/>
-      <c r="M4" s="51"/>
-      <c r="N4" s="52"/>
-      <c r="P4" s="60" t="s">
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61"/>
+      <c r="M4" s="61"/>
+      <c r="N4" s="62"/>
+      <c r="P4" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="Q4" s="51"/>
-      <c r="R4" s="51"/>
-      <c r="S4" s="51"/>
-      <c r="T4" s="51"/>
-      <c r="U4" s="52"/>
-      <c r="W4" s="59" t="s">
+      <c r="Q4" s="61"/>
+      <c r="R4" s="61"/>
+      <c r="S4" s="61"/>
+      <c r="T4" s="61"/>
+      <c r="U4" s="62"/>
+      <c r="W4" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="X4" s="51"/>
-      <c r="Y4" s="51"/>
-      <c r="Z4" s="51"/>
-      <c r="AA4" s="51"/>
-      <c r="AB4" s="52"/>
+      <c r="X4" s="61"/>
+      <c r="Y4" s="61"/>
+      <c r="Z4" s="61"/>
+      <c r="AA4" s="61"/>
+      <c r="AB4" s="62"/>
     </row>
     <row r="5" spans="2:28" ht="14.25" customHeight="1">
       <c r="B5" s="26" t="s">
@@ -4220,38 +4432,38 @@
     <row r="15" spans="2:28" ht="14.25" customHeight="1"/>
     <row r="16" spans="2:28" ht="14.25" customHeight="1"/>
     <row r="17" spans="2:28" ht="14.25" customHeight="1">
-      <c r="B17" s="63" t="s">
+      <c r="B17" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="51"/>
-      <c r="D17" s="51"/>
-      <c r="E17" s="51"/>
-      <c r="F17" s="51"/>
-      <c r="G17" s="52"/>
-      <c r="I17" s="58" t="s">
+      <c r="C17" s="61"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="61"/>
+      <c r="F17" s="61"/>
+      <c r="G17" s="62"/>
+      <c r="I17" s="68" t="s">
         <v>75</v>
       </c>
-      <c r="J17" s="51"/>
-      <c r="K17" s="51"/>
-      <c r="L17" s="51"/>
-      <c r="M17" s="51"/>
-      <c r="N17" s="52"/>
-      <c r="P17" s="54" t="s">
+      <c r="J17" s="61"/>
+      <c r="K17" s="61"/>
+      <c r="L17" s="61"/>
+      <c r="M17" s="61"/>
+      <c r="N17" s="62"/>
+      <c r="P17" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="Q17" s="51"/>
-      <c r="R17" s="51"/>
-      <c r="S17" s="51"/>
-      <c r="T17" s="51"/>
-      <c r="U17" s="52"/>
-      <c r="W17" s="66" t="s">
+      <c r="Q17" s="61"/>
+      <c r="R17" s="61"/>
+      <c r="S17" s="61"/>
+      <c r="T17" s="61"/>
+      <c r="U17" s="62"/>
+      <c r="W17" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="X17" s="51"/>
-      <c r="Y17" s="51"/>
-      <c r="Z17" s="51"/>
-      <c r="AA17" s="51"/>
-      <c r="AB17" s="52"/>
+      <c r="X17" s="61"/>
+      <c r="Y17" s="61"/>
+      <c r="Z17" s="61"/>
+      <c r="AA17" s="61"/>
+      <c r="AB17" s="62"/>
     </row>
     <row r="18" spans="2:28" ht="14.25" customHeight="1">
       <c r="B18" s="26" t="s">
@@ -5641,8 +5853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B1:I1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:H62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -5660,80 +5872,80 @@
     <row r="1" spans="2:8" ht="14.25" customHeight="1"/>
     <row r="2" spans="2:8" ht="14.25" customHeight="1"/>
     <row r="3" spans="2:8" ht="14.25" customHeight="1">
-      <c r="B3" s="66" t="s">
+      <c r="B3" s="76" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="51"/>
-      <c r="D3" s="51"/>
-      <c r="E3" s="51"/>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="52"/>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="62"/>
     </row>
     <row r="4" spans="2:8" ht="14.25" customHeight="1">
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="77" t="s">
         <v>78</v>
       </c>
-      <c r="C4" s="52"/>
+      <c r="C4" s="62"/>
       <c r="D4" s="29" t="s">
         <v>76</v>
       </c>
       <c r="E4" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="F4" s="55" t="s">
+      <c r="F4" s="65" t="s">
         <v>55</v>
       </c>
-      <c r="G4" s="51"/>
-      <c r="H4" s="52"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="62"/>
     </row>
     <row r="5" spans="2:8" ht="14.25" customHeight="1">
-      <c r="B5" s="69">
+      <c r="B5" s="79">
         <v>1</v>
       </c>
-      <c r="C5" s="52"/>
+      <c r="C5" s="62"/>
       <c r="D5" s="37" t="s">
         <v>109</v>
       </c>
       <c r="E5" s="36">
         <v>5</v>
       </c>
-      <c r="F5" s="74">
+      <c r="F5" s="84">
         <v>44811</v>
       </c>
-      <c r="G5" s="51"/>
-      <c r="H5" s="52"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="62"/>
     </row>
     <row r="6" spans="2:8" ht="14.25" customHeight="1">
-      <c r="B6" s="69"/>
-      <c r="C6" s="52"/>
+      <c r="B6" s="79"/>
+      <c r="C6" s="62"/>
       <c r="D6" s="39"/>
       <c r="E6" s="38"/>
-      <c r="F6" s="69"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="52"/>
+      <c r="F6" s="79"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="62"/>
     </row>
     <row r="7" spans="2:8" ht="14.25" customHeight="1">
-      <c r="B7" s="69"/>
-      <c r="C7" s="52"/>
+      <c r="B7" s="79"/>
+      <c r="C7" s="62"/>
       <c r="D7" s="39"/>
       <c r="E7" s="38"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="52"/>
+      <c r="F7" s="79"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="62"/>
     </row>
     <row r="8" spans="2:8" ht="14.25" customHeight="1"/>
     <row r="9" spans="2:8" ht="14.25" customHeight="1"/>
     <row r="10" spans="2:8" ht="14.25" customHeight="1">
-      <c r="B10" s="65" t="s">
+      <c r="B10" s="75" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
-      <c r="G10" s="51"/>
-      <c r="H10" s="52"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="61"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="61"/>
+      <c r="H10" s="62"/>
     </row>
     <row r="11" spans="2:8" ht="14.25" customHeight="1">
       <c r="B11" s="24" t="s">
@@ -5751,10 +5963,10 @@
       <c r="F11" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="G11" s="55" t="s">
+      <c r="G11" s="65" t="s">
         <v>80</v>
       </c>
-      <c r="H11" s="52"/>
+      <c r="H11" s="62"/>
     </row>
     <row r="12" spans="2:8" ht="14.25" customHeight="1">
       <c r="B12" s="40" t="s">
@@ -5772,10 +5984,10 @@
       <c r="F12" s="41">
         <v>44445858</v>
       </c>
-      <c r="G12" s="69" t="s">
+      <c r="G12" s="79" t="s">
         <v>53</v>
       </c>
-      <c r="H12" s="52"/>
+      <c r="H12" s="62"/>
     </row>
     <row r="13" spans="2:8" ht="14.25" customHeight="1">
       <c r="B13" s="41"/>
@@ -5783,30 +5995,30 @@
       <c r="D13" s="41"/>
       <c r="E13" s="41"/>
       <c r="F13" s="41"/>
-      <c r="G13" s="69"/>
-      <c r="H13" s="52"/>
+      <c r="G13" s="79"/>
+      <c r="H13" s="62"/>
     </row>
     <row r="14" spans="2:8" ht="14.25" customHeight="1"/>
     <row r="15" spans="2:8" ht="14.25" customHeight="1"/>
     <row r="16" spans="2:8" ht="14.25" customHeight="1">
-      <c r="B16" s="50" t="s">
+      <c r="B16" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="51"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="51"/>
-      <c r="F16" s="51"/>
-      <c r="G16" s="51"/>
-      <c r="H16" s="52"/>
+      <c r="C16" s="61"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="61"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="61"/>
+      <c r="H16" s="62"/>
     </row>
     <row r="17" spans="2:9" ht="14.25" customHeight="1">
       <c r="B17" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="C17" s="72" t="s">
+      <c r="C17" s="82" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="52"/>
+      <c r="D17" s="62"/>
       <c r="E17" s="26" t="s">
         <v>72</v>
       </c>
@@ -5824,10 +6036,10 @@
       <c r="B18" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="C18" s="69" t="s">
+      <c r="C18" s="79" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="52"/>
+      <c r="D18" s="62"/>
       <c r="E18" s="44">
         <v>28332</v>
       </c>
@@ -5843,9 +6055,9 @@
     </row>
     <row r="19" spans="2:9" ht="14.25" customHeight="1">
       <c r="B19" s="45"/>
-      <c r="C19" s="68"/>
-      <c r="D19" s="52"/>
-      <c r="E19" s="46"/>
+      <c r="C19" s="78"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="47"/>
       <c r="F19" s="41"/>
       <c r="G19" s="41"/>
       <c r="H19" s="41"/>
@@ -5853,18 +6065,18 @@
     </row>
     <row r="20" spans="2:9" ht="14.25" customHeight="1">
       <c r="B20" s="45"/>
-      <c r="C20" s="68"/>
-      <c r="D20" s="52"/>
-      <c r="E20" s="46"/>
+      <c r="C20" s="78"/>
+      <c r="D20" s="62"/>
+      <c r="E20" s="47"/>
       <c r="F20" s="41"/>
       <c r="G20" s="41"/>
       <c r="H20" s="41"/>
     </row>
     <row r="21" spans="2:9" ht="14.25" customHeight="1">
       <c r="B21" s="45"/>
-      <c r="C21" s="68"/>
-      <c r="D21" s="52"/>
-      <c r="E21" s="46"/>
+      <c r="C21" s="78"/>
+      <c r="D21" s="62"/>
+      <c r="E21" s="47"/>
       <c r="F21" s="41"/>
       <c r="G21" s="41"/>
       <c r="H21" s="41"/>
@@ -5872,15 +6084,15 @@
     <row r="22" spans="2:9" ht="14.25" customHeight="1"/>
     <row r="23" spans="2:9" ht="14.25" customHeight="1"/>
     <row r="24" spans="2:9" ht="14.25" customHeight="1">
-      <c r="B24" s="58" t="s">
+      <c r="B24" s="68" t="s">
         <v>75</v>
       </c>
-      <c r="C24" s="51"/>
-      <c r="D24" s="51"/>
-      <c r="E24" s="51"/>
-      <c r="F24" s="51"/>
-      <c r="G24" s="51"/>
-      <c r="H24" s="52"/>
+      <c r="C24" s="61"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="61"/>
+      <c r="F24" s="61"/>
+      <c r="G24" s="61"/>
+      <c r="H24" s="62"/>
     </row>
     <row r="25" spans="2:9" ht="14.25" customHeight="1">
       <c r="B25" s="24" t="s">
@@ -5895,11 +6107,11 @@
       <c r="E25" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="F25" s="73" t="s">
+      <c r="F25" s="83" t="s">
         <v>55</v>
       </c>
-      <c r="G25" s="51"/>
-      <c r="H25" s="52"/>
+      <c r="G25" s="61"/>
+      <c r="H25" s="62"/>
     </row>
     <row r="26" spans="2:9" ht="14.25" customHeight="1">
       <c r="B26" s="40" t="s">
@@ -5914,11 +6126,11 @@
       <c r="E26" s="41" t="s">
         <v>116</v>
       </c>
-      <c r="F26" s="74">
+      <c r="F26" s="84">
         <v>44811</v>
       </c>
-      <c r="G26" s="51"/>
-      <c r="H26" s="52"/>
+      <c r="G26" s="61"/>
+      <c r="H26" s="62"/>
     </row>
     <row r="27" spans="2:9" ht="14.25" customHeight="1">
       <c r="B27" s="40" t="s">
@@ -5933,33 +6145,33 @@
       <c r="E27" s="41" t="s">
         <v>119</v>
       </c>
-      <c r="F27" s="74">
+      <c r="F27" s="84">
         <v>44788</v>
       </c>
-      <c r="G27" s="51"/>
-      <c r="H27" s="52"/>
+      <c r="G27" s="61"/>
+      <c r="H27" s="62"/>
     </row>
     <row r="28" spans="2:9" ht="14.25" customHeight="1">
       <c r="B28" s="45"/>
       <c r="C28" s="41"/>
       <c r="D28" s="41"/>
-      <c r="E28" s="69"/>
-      <c r="F28" s="51"/>
-      <c r="G28" s="51"/>
-      <c r="H28" s="52"/>
+      <c r="E28" s="79"/>
+      <c r="F28" s="61"/>
+      <c r="G28" s="61"/>
+      <c r="H28" s="62"/>
     </row>
     <row r="29" spans="2:9" ht="14.25" customHeight="1"/>
     <row r="30" spans="2:9" ht="14.25" customHeight="1"/>
     <row r="31" spans="2:9" ht="14.25" customHeight="1">
-      <c r="B31" s="59" t="s">
+      <c r="B31" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="C31" s="51"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="51"/>
-      <c r="F31" s="51"/>
-      <c r="G31" s="51"/>
-      <c r="H31" s="52"/>
+      <c r="C31" s="61"/>
+      <c r="D31" s="61"/>
+      <c r="E31" s="61"/>
+      <c r="F31" s="61"/>
+      <c r="G31" s="61"/>
+      <c r="H31" s="62"/>
     </row>
     <row r="32" spans="2:9" ht="14.25" customHeight="1">
       <c r="B32" s="24" t="s">
@@ -5971,15 +6183,15 @@
       <c r="D32" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="E32" s="55" t="s">
+      <c r="E32" s="65" t="s">
         <v>25</v>
       </c>
-      <c r="F32" s="51"/>
-      <c r="G32" s="51"/>
-      <c r="H32" s="52"/>
+      <c r="F32" s="61"/>
+      <c r="G32" s="61"/>
+      <c r="H32" s="62"/>
     </row>
     <row r="33" spans="2:8" ht="14.25" customHeight="1">
-      <c r="B33" s="75">
+      <c r="B33" s="85">
         <v>344</v>
       </c>
       <c r="C33" s="41">
@@ -5988,85 +6200,85 @@
       <c r="D33" s="41">
         <v>2</v>
       </c>
-      <c r="E33" s="71">
+      <c r="E33" s="81">
         <v>10000</v>
       </c>
-      <c r="F33" s="51"/>
-      <c r="G33" s="51"/>
-      <c r="H33" s="52"/>
+      <c r="F33" s="61"/>
+      <c r="G33" s="61"/>
+      <c r="H33" s="62"/>
     </row>
     <row r="34" spans="2:8" ht="14.25" customHeight="1">
-      <c r="B34" s="76"/>
+      <c r="B34" s="86"/>
       <c r="C34" s="41">
         <v>29</v>
       </c>
       <c r="D34" s="41">
         <v>5</v>
       </c>
-      <c r="E34" s="71">
+      <c r="E34" s="81">
         <v>15000</v>
       </c>
-      <c r="F34" s="51"/>
-      <c r="G34" s="51"/>
-      <c r="H34" s="52"/>
+      <c r="F34" s="61"/>
+      <c r="G34" s="61"/>
+      <c r="H34" s="62"/>
     </row>
     <row r="35" spans="2:8" ht="14.25" customHeight="1">
-      <c r="B35" s="76"/>
+      <c r="B35" s="86"/>
       <c r="C35" s="41">
         <v>87</v>
       </c>
       <c r="D35" s="41">
         <v>1</v>
       </c>
-      <c r="E35" s="71">
+      <c r="E35" s="81">
         <v>15000</v>
       </c>
-      <c r="F35" s="51"/>
-      <c r="G35" s="51"/>
-      <c r="H35" s="52"/>
+      <c r="F35" s="61"/>
+      <c r="G35" s="61"/>
+      <c r="H35" s="62"/>
     </row>
     <row r="36" spans="2:8" ht="14.25" customHeight="1">
-      <c r="B36" s="76"/>
+      <c r="B36" s="86"/>
       <c r="C36" s="41">
         <v>36</v>
       </c>
       <c r="D36" s="41">
         <v>3</v>
       </c>
-      <c r="E36" s="71">
+      <c r="E36" s="81">
         <v>22500</v>
       </c>
-      <c r="F36" s="51"/>
-      <c r="G36" s="51"/>
-      <c r="H36" s="52"/>
+      <c r="F36" s="61"/>
+      <c r="G36" s="61"/>
+      <c r="H36" s="62"/>
     </row>
     <row r="37" spans="2:8" ht="14.25" customHeight="1">
-      <c r="B37" s="77"/>
+      <c r="B37" s="87"/>
       <c r="C37" s="41">
         <v>89</v>
       </c>
       <c r="D37" s="41">
         <v>7</v>
       </c>
-      <c r="E37" s="71">
+      <c r="E37" s="81">
         <v>7000</v>
       </c>
-      <c r="F37" s="51"/>
-      <c r="G37" s="51"/>
-      <c r="H37" s="52"/>
+      <c r="F37" s="61"/>
+      <c r="G37" s="61"/>
+      <c r="H37" s="62"/>
     </row>
     <row r="38" spans="2:8" ht="14.25" customHeight="1"/>
     <row r="39" spans="2:8" ht="14.25" customHeight="1"/>
     <row r="40" spans="2:8" ht="14.25" customHeight="1">
-      <c r="B40" s="54" t="s">
+      <c r="B40" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="C40" s="51"/>
-      <c r="D40" s="51"/>
-      <c r="E40" s="51"/>
-      <c r="F40" s="51"/>
-      <c r="G40" s="51"/>
-      <c r="H40" s="52"/>
+      <c r="C40" s="61"/>
+      <c r="D40" s="61"/>
+      <c r="E40" s="61"/>
+      <c r="F40" s="61"/>
+      <c r="G40" s="61"/>
+      <c r="H40" s="62"/>
     </row>
     <row r="41" spans="2:8" ht="14.25" customHeight="1">
       <c r="B41" s="24" t="s">
@@ -6078,226 +6290,226 @@
       <c r="D41" s="27" t="s">
         <v>45</v>
       </c>
-      <c r="E41" s="55" t="s">
+      <c r="E41" s="65" t="s">
         <v>51</v>
       </c>
-      <c r="F41" s="51"/>
-      <c r="G41" s="51"/>
-      <c r="H41" s="52"/>
+      <c r="F41" s="61"/>
+      <c r="G41" s="61"/>
+      <c r="H41" s="62"/>
     </row>
     <row r="42" spans="2:8" ht="14.25" customHeight="1">
-      <c r="B42" s="47">
+      <c r="B42" s="48">
         <v>54</v>
       </c>
-      <c r="C42" s="48">
+      <c r="C42" s="49">
         <v>5000</v>
       </c>
       <c r="D42" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="E42" s="69" t="s">
+      <c r="E42" s="79" t="s">
         <v>62</v>
       </c>
-      <c r="F42" s="51"/>
-      <c r="G42" s="51"/>
-      <c r="H42" s="52"/>
+      <c r="F42" s="61"/>
+      <c r="G42" s="61"/>
+      <c r="H42" s="62"/>
     </row>
     <row r="43" spans="2:8" ht="14.25" customHeight="1">
-      <c r="B43" s="47">
+      <c r="B43" s="48">
         <v>29</v>
       </c>
-      <c r="C43" s="48">
+      <c r="C43" s="49">
         <v>3000</v>
       </c>
       <c r="D43" s="41" t="s">
         <v>120</v>
       </c>
-      <c r="E43" s="69" t="s">
+      <c r="E43" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="F43" s="51"/>
-      <c r="G43" s="51"/>
-      <c r="H43" s="52"/>
+      <c r="F43" s="61"/>
+      <c r="G43" s="61"/>
+      <c r="H43" s="62"/>
     </row>
     <row r="44" spans="2:8" ht="14.25" customHeight="1">
-      <c r="B44" s="47">
+      <c r="B44" s="48">
         <v>87</v>
       </c>
-      <c r="C44" s="48">
+      <c r="C44" s="49">
         <v>15000</v>
       </c>
       <c r="D44" s="41" t="s">
         <v>121</v>
       </c>
-      <c r="E44" s="69" t="s">
+      <c r="E44" s="79" t="s">
         <v>122</v>
       </c>
-      <c r="F44" s="51"/>
-      <c r="G44" s="51"/>
-      <c r="H44" s="52"/>
+      <c r="F44" s="61"/>
+      <c r="G44" s="61"/>
+      <c r="H44" s="62"/>
     </row>
     <row r="45" spans="2:8" ht="14.25" customHeight="1">
-      <c r="B45" s="47">
+      <c r="B45" s="48">
         <v>36</v>
       </c>
-      <c r="C45" s="48">
+      <c r="C45" s="49">
         <v>7500</v>
       </c>
       <c r="D45" s="41" t="s">
         <v>123</v>
       </c>
-      <c r="E45" s="69" t="s">
+      <c r="E45" s="79" t="s">
         <v>30</v>
       </c>
-      <c r="F45" s="51"/>
-      <c r="G45" s="51"/>
-      <c r="H45" s="52"/>
+      <c r="F45" s="61"/>
+      <c r="G45" s="61"/>
+      <c r="H45" s="62"/>
     </row>
     <row r="46" spans="2:8" ht="14.25" customHeight="1">
-      <c r="B46" s="47">
+      <c r="B46" s="48">
         <v>89</v>
       </c>
-      <c r="C46" s="48">
+      <c r="C46" s="49">
         <v>1000</v>
       </c>
       <c r="D46" s="41" t="s">
         <v>124</v>
       </c>
-      <c r="E46" s="69" t="s">
+      <c r="E46" s="79" t="s">
         <v>46</v>
       </c>
-      <c r="F46" s="51"/>
-      <c r="G46" s="51"/>
-      <c r="H46" s="52"/>
+      <c r="F46" s="61"/>
+      <c r="G46" s="61"/>
+      <c r="H46" s="62"/>
     </row>
     <row r="47" spans="2:8" ht="14.25" customHeight="1">
       <c r="B47" s="41"/>
       <c r="C47" s="41"/>
       <c r="D47" s="41"/>
-      <c r="E47" s="69"/>
-      <c r="F47" s="51"/>
-      <c r="G47" s="51"/>
-      <c r="H47" s="52"/>
+      <c r="E47" s="79"/>
+      <c r="F47" s="61"/>
+      <c r="G47" s="61"/>
+      <c r="H47" s="62"/>
     </row>
     <row r="48" spans="2:8" ht="14.25" customHeight="1"/>
     <row r="49" spans="2:8" ht="14.25" customHeight="1"/>
     <row r="50" spans="2:8" ht="14.25" customHeight="1">
-      <c r="B50" s="63" t="s">
+      <c r="B50" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="C50" s="51"/>
-      <c r="D50" s="51"/>
-      <c r="E50" s="51"/>
-      <c r="F50" s="51"/>
-      <c r="G50" s="51"/>
-      <c r="H50" s="52"/>
+      <c r="C50" s="61"/>
+      <c r="D50" s="61"/>
+      <c r="E50" s="61"/>
+      <c r="F50" s="61"/>
+      <c r="G50" s="61"/>
+      <c r="H50" s="62"/>
     </row>
     <row r="51" spans="2:8" ht="14.25" customHeight="1">
-      <c r="B51" s="64" t="s">
+      <c r="B51" s="74" t="s">
         <v>77</v>
       </c>
-      <c r="C51" s="51"/>
-      <c r="D51" s="51"/>
-      <c r="E51" s="51"/>
-      <c r="F51" s="51"/>
-      <c r="G51" s="51"/>
-      <c r="H51" s="52"/>
+      <c r="C51" s="61"/>
+      <c r="D51" s="61"/>
+      <c r="E51" s="61"/>
+      <c r="F51" s="61"/>
+      <c r="G51" s="61"/>
+      <c r="H51" s="62"/>
     </row>
     <row r="52" spans="2:8" ht="14.25" customHeight="1">
-      <c r="B52" s="69">
+      <c r="B52" s="79">
         <v>1</v>
       </c>
-      <c r="C52" s="51"/>
-      <c r="D52" s="51"/>
-      <c r="E52" s="51"/>
-      <c r="F52" s="51"/>
-      <c r="G52" s="51"/>
-      <c r="H52" s="52"/>
+      <c r="C52" s="61"/>
+      <c r="D52" s="61"/>
+      <c r="E52" s="61"/>
+      <c r="F52" s="61"/>
+      <c r="G52" s="61"/>
+      <c r="H52" s="62"/>
     </row>
     <row r="53" spans="2:8" ht="14.25" customHeight="1">
-      <c r="B53" s="69">
+      <c r="B53" s="79">
         <v>2</v>
       </c>
-      <c r="C53" s="51"/>
-      <c r="D53" s="51"/>
-      <c r="E53" s="51"/>
-      <c r="F53" s="51"/>
-      <c r="G53" s="51"/>
-      <c r="H53" s="52"/>
+      <c r="C53" s="61"/>
+      <c r="D53" s="61"/>
+      <c r="E53" s="61"/>
+      <c r="F53" s="61"/>
+      <c r="G53" s="61"/>
+      <c r="H53" s="62"/>
     </row>
     <row r="54" spans="2:8" ht="14.25" customHeight="1">
-      <c r="B54" s="69"/>
-      <c r="C54" s="51"/>
-      <c r="D54" s="51"/>
-      <c r="E54" s="51"/>
-      <c r="F54" s="51"/>
-      <c r="G54" s="51"/>
-      <c r="H54" s="52"/>
+      <c r="B54" s="79"/>
+      <c r="C54" s="61"/>
+      <c r="D54" s="61"/>
+      <c r="E54" s="61"/>
+      <c r="F54" s="61"/>
+      <c r="G54" s="61"/>
+      <c r="H54" s="62"/>
     </row>
     <row r="55" spans="2:8" ht="14.25" customHeight="1"/>
     <row r="56" spans="2:8" ht="14.25" customHeight="1"/>
     <row r="57" spans="2:8" ht="14.25" customHeight="1">
-      <c r="B57" s="60" t="s">
+      <c r="B57" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="C57" s="51"/>
-      <c r="D57" s="51"/>
-      <c r="E57" s="51"/>
-      <c r="F57" s="51"/>
-      <c r="G57" s="51"/>
-      <c r="H57" s="52"/>
+      <c r="C57" s="61"/>
+      <c r="D57" s="61"/>
+      <c r="E57" s="61"/>
+      <c r="F57" s="61"/>
+      <c r="G57" s="61"/>
+      <c r="H57" s="62"/>
     </row>
     <row r="58" spans="2:8" ht="14.25" customHeight="1">
-      <c r="B58" s="61" t="s">
+      <c r="B58" s="71" t="s">
         <v>81</v>
       </c>
-      <c r="C58" s="52"/>
+      <c r="C58" s="62"/>
       <c r="D58" s="27" t="s">
         <v>19</v>
       </c>
       <c r="E58" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="F58" s="62" t="s">
+      <c r="F58" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="G58" s="51"/>
-      <c r="H58" s="52"/>
+      <c r="G58" s="61"/>
+      <c r="H58" s="62"/>
     </row>
     <row r="59" spans="2:8" ht="14.25" customHeight="1">
-      <c r="B59" s="70">
+      <c r="B59" s="80">
         <v>344</v>
       </c>
-      <c r="C59" s="52"/>
-      <c r="D59" s="48">
+      <c r="C59" s="62"/>
+      <c r="D59" s="49">
         <v>69500</v>
       </c>
       <c r="E59" s="41">
         <v>0.19</v>
       </c>
-      <c r="F59" s="71">
+      <c r="F59" s="81">
         <v>82705</v>
       </c>
-      <c r="G59" s="51"/>
-      <c r="H59" s="52"/>
+      <c r="G59" s="61"/>
+      <c r="H59" s="62"/>
     </row>
     <row r="60" spans="2:8" ht="14.25" customHeight="1">
-      <c r="B60" s="68"/>
-      <c r="C60" s="52"/>
+      <c r="B60" s="78"/>
+      <c r="C60" s="62"/>
       <c r="D60" s="41"/>
       <c r="E60" s="41"/>
-      <c r="F60" s="69"/>
-      <c r="G60" s="51"/>
-      <c r="H60" s="52"/>
+      <c r="F60" s="79"/>
+      <c r="G60" s="61"/>
+      <c r="H60" s="62"/>
     </row>
     <row r="61" spans="2:8" ht="14.25" customHeight="1">
-      <c r="B61" s="68"/>
-      <c r="C61" s="52"/>
+      <c r="B61" s="78"/>
+      <c r="C61" s="62"/>
       <c r="D61" s="41"/>
       <c r="E61" s="41"/>
-      <c r="F61" s="69"/>
-      <c r="G61" s="51"/>
-      <c r="H61" s="52"/>
+      <c r="F61" s="79"/>
+      <c r="G61" s="61"/>
+      <c r="H61" s="62"/>
     </row>
     <row r="62" spans="2:8" ht="14.25" customHeight="1"/>
     <row r="63" spans="2:8" ht="14.25" customHeight="1"/>
@@ -6306,7 +6518,7 @@
       <c r="I65" s="32"/>
     </row>
     <row r="66" spans="9:9" ht="14.25" customHeight="1">
-      <c r="I66" s="49"/>
+      <c r="I66" s="50"/>
     </row>
     <row r="67" spans="9:9" ht="14.25" customHeight="1">
       <c r="I67" s="28"/>
@@ -7313,4 +7525,694 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48449349-DB66-431B-AB82-758E76C2233B}">
+  <dimension ref="B2:Q24"/>
+  <sheetViews>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="15.28515625" customWidth="1"/>
+    <col min="7" max="7" width="14.5703125" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:17">
+      <c r="I2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="4" spans="2:17">
+      <c r="B4" s="64" t="s">
+        <v>125</v>
+      </c>
+      <c r="C4" s="61"/>
+      <c r="D4" s="61"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="62"/>
+      <c r="K4" s="69" t="s">
+        <v>126</v>
+      </c>
+      <c r="L4" s="61"/>
+      <c r="M4" s="61"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="61"/>
+      <c r="P4" s="61"/>
+      <c r="Q4" s="62"/>
+    </row>
+    <row r="5" spans="2:17">
+      <c r="B5" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="C5" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="65" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="61"/>
+      <c r="G5" s="61"/>
+      <c r="H5" s="62"/>
+      <c r="K5" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="L5" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="M5" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="N5" s="65" t="s">
+        <v>25</v>
+      </c>
+      <c r="O5" s="61"/>
+      <c r="P5" s="61"/>
+      <c r="Q5" s="62"/>
+    </row>
+    <row r="6" spans="2:17">
+      <c r="B6" s="48">
+        <v>54</v>
+      </c>
+      <c r="C6" s="49">
+        <v>5000</v>
+      </c>
+      <c r="D6" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="79" t="s">
+        <v>62</v>
+      </c>
+      <c r="F6" s="61"/>
+      <c r="G6" s="61"/>
+      <c r="H6" s="62"/>
+      <c r="K6" s="85">
+        <v>344</v>
+      </c>
+      <c r="L6" s="41">
+        <v>54</v>
+      </c>
+      <c r="M6" s="41">
+        <v>2</v>
+      </c>
+      <c r="N6" s="81">
+        <v>10000</v>
+      </c>
+      <c r="O6" s="61"/>
+      <c r="P6" s="61"/>
+      <c r="Q6" s="62"/>
+    </row>
+    <row r="7" spans="2:17">
+      <c r="B7" s="48">
+        <v>29</v>
+      </c>
+      <c r="C7" s="49">
+        <v>3000</v>
+      </c>
+      <c r="D7" s="41" t="s">
+        <v>120</v>
+      </c>
+      <c r="E7" s="79" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="62"/>
+      <c r="K7" s="86"/>
+      <c r="L7" s="41">
+        <v>29</v>
+      </c>
+      <c r="M7" s="41">
+        <v>5</v>
+      </c>
+      <c r="N7" s="81">
+        <v>15000</v>
+      </c>
+      <c r="O7" s="61"/>
+      <c r="P7" s="61"/>
+      <c r="Q7" s="62"/>
+    </row>
+    <row r="8" spans="2:17">
+      <c r="B8" s="48">
+        <v>87</v>
+      </c>
+      <c r="C8" s="49">
+        <v>15000</v>
+      </c>
+      <c r="D8" s="41" t="s">
+        <v>121</v>
+      </c>
+      <c r="E8" s="79" t="s">
+        <v>122</v>
+      </c>
+      <c r="F8" s="61"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="62"/>
+      <c r="K8" s="86"/>
+      <c r="L8" s="41">
+        <v>87</v>
+      </c>
+      <c r="M8" s="41">
+        <v>1</v>
+      </c>
+      <c r="N8" s="81">
+        <v>15000</v>
+      </c>
+      <c r="O8" s="61"/>
+      <c r="P8" s="61"/>
+      <c r="Q8" s="62"/>
+    </row>
+    <row r="9" spans="2:17">
+      <c r="B9" s="48">
+        <v>36</v>
+      </c>
+      <c r="C9" s="49">
+        <v>7500</v>
+      </c>
+      <c r="D9" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="E9" s="79" t="s">
+        <v>30</v>
+      </c>
+      <c r="F9" s="61"/>
+      <c r="G9" s="61"/>
+      <c r="H9" s="62"/>
+      <c r="K9" s="86"/>
+      <c r="L9" s="41">
+        <v>36</v>
+      </c>
+      <c r="M9" s="41">
+        <v>3</v>
+      </c>
+      <c r="N9" s="81">
+        <v>22500</v>
+      </c>
+      <c r="O9" s="61"/>
+      <c r="P9" s="61"/>
+      <c r="Q9" s="62"/>
+    </row>
+    <row r="10" spans="2:17">
+      <c r="B10" s="48">
+        <v>89</v>
+      </c>
+      <c r="C10" s="49">
+        <v>1000</v>
+      </c>
+      <c r="D10" s="41" t="s">
+        <v>124</v>
+      </c>
+      <c r="E10" s="79" t="s">
+        <v>46</v>
+      </c>
+      <c r="F10" s="61"/>
+      <c r="G10" s="61"/>
+      <c r="H10" s="62"/>
+      <c r="K10" s="87"/>
+      <c r="L10" s="41">
+        <v>89</v>
+      </c>
+      <c r="M10" s="41">
+        <v>7</v>
+      </c>
+      <c r="N10" s="81">
+        <v>7000</v>
+      </c>
+      <c r="O10" s="61"/>
+      <c r="P10" s="61"/>
+      <c r="Q10" s="62"/>
+    </row>
+    <row r="11" spans="2:17">
+      <c r="B11" s="41"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="79"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="61"/>
+      <c r="H11" s="62"/>
+    </row>
+    <row r="13" spans="2:17">
+      <c r="G13" s="91" t="s">
+        <v>133</v>
+      </c>
+      <c r="H13" s="92"/>
+      <c r="I13" s="92"/>
+      <c r="J13" s="92"/>
+      <c r="K13" s="92"/>
+      <c r="L13" s="92"/>
+      <c r="M13" s="92"/>
+      <c r="N13" s="93"/>
+    </row>
+    <row r="14" spans="2:17">
+      <c r="G14" s="91" t="s">
+        <v>132</v>
+      </c>
+      <c r="H14" s="92"/>
+      <c r="I14" s="92"/>
+      <c r="J14" s="92"/>
+      <c r="K14" s="92"/>
+      <c r="L14" s="92"/>
+      <c r="M14" s="92"/>
+      <c r="N14" s="93"/>
+    </row>
+    <row r="15" spans="2:17">
+      <c r="G15" s="52" t="s">
+        <v>127</v>
+      </c>
+      <c r="H15" s="53" t="s">
+        <v>128</v>
+      </c>
+      <c r="I15" s="54" t="s">
+        <v>130</v>
+      </c>
+      <c r="J15" s="54" t="s">
+        <v>131</v>
+      </c>
+      <c r="K15" s="88" t="s">
+        <v>129</v>
+      </c>
+      <c r="L15" s="89"/>
+      <c r="M15" s="89"/>
+      <c r="N15" s="90"/>
+    </row>
+    <row r="16" spans="2:17">
+      <c r="G16" s="48">
+        <v>54</v>
+      </c>
+      <c r="H16" s="46">
+        <v>54</v>
+      </c>
+      <c r="I16" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="J16" s="56">
+        <v>5000</v>
+      </c>
+      <c r="K16" s="81">
+        <v>10000</v>
+      </c>
+      <c r="L16" s="61"/>
+      <c r="M16" s="61"/>
+      <c r="N16" s="62"/>
+    </row>
+    <row r="17" spans="2:14">
+      <c r="G17" s="48">
+        <v>29</v>
+      </c>
+      <c r="H17" s="46">
+        <v>29</v>
+      </c>
+      <c r="I17" s="55" t="s">
+        <v>37</v>
+      </c>
+      <c r="J17" s="56">
+        <v>3000</v>
+      </c>
+      <c r="K17" s="81">
+        <v>15000</v>
+      </c>
+      <c r="L17" s="61"/>
+      <c r="M17" s="61"/>
+      <c r="N17" s="62"/>
+    </row>
+    <row r="18" spans="2:14">
+      <c r="G18" s="48">
+        <v>87</v>
+      </c>
+      <c r="H18" s="46">
+        <v>87</v>
+      </c>
+      <c r="I18" s="55" t="s">
+        <v>122</v>
+      </c>
+      <c r="J18" s="56">
+        <v>15000</v>
+      </c>
+      <c r="K18" s="81">
+        <v>15000</v>
+      </c>
+      <c r="L18" s="61"/>
+      <c r="M18" s="61"/>
+      <c r="N18" s="62"/>
+    </row>
+    <row r="19" spans="2:14">
+      <c r="G19" s="48">
+        <v>36</v>
+      </c>
+      <c r="H19" s="46">
+        <v>36</v>
+      </c>
+      <c r="I19" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="J19" s="56">
+        <v>7500</v>
+      </c>
+      <c r="K19" s="81">
+        <v>22500</v>
+      </c>
+      <c r="L19" s="61"/>
+      <c r="M19" s="61"/>
+      <c r="N19" s="62"/>
+    </row>
+    <row r="20" spans="2:14">
+      <c r="G20" s="48">
+        <v>89</v>
+      </c>
+      <c r="H20" s="46">
+        <v>89</v>
+      </c>
+      <c r="I20" s="55" t="s">
+        <v>46</v>
+      </c>
+      <c r="J20" s="56">
+        <v>1000</v>
+      </c>
+      <c r="K20" s="81">
+        <v>7000</v>
+      </c>
+      <c r="L20" s="61"/>
+      <c r="M20" s="61"/>
+      <c r="N20" s="62"/>
+    </row>
+    <row r="24" spans="2:14">
+      <c r="B24" s="57"/>
+    </row>
+  </sheetData>
+  <mergeCells count="24">
+    <mergeCell ref="K16:N16"/>
+    <mergeCell ref="K17:N17"/>
+    <mergeCell ref="K18:N18"/>
+    <mergeCell ref="K19:N19"/>
+    <mergeCell ref="K20:N20"/>
+    <mergeCell ref="K15:N15"/>
+    <mergeCell ref="G14:N14"/>
+    <mergeCell ref="G13:N13"/>
+    <mergeCell ref="E10:H10"/>
+    <mergeCell ref="E11:H11"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="N5:Q5"/>
+    <mergeCell ref="K6:K10"/>
+    <mergeCell ref="N6:Q6"/>
+    <mergeCell ref="N7:Q7"/>
+    <mergeCell ref="N8:Q8"/>
+    <mergeCell ref="N9:Q9"/>
+    <mergeCell ref="N10:Q10"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="E5:H5"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="E8:H8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62E844BE-1773-4350-A231-8236468899CC}">
+  <dimension ref="B3:Q18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="5" max="5" width="26" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="10" customWidth="1"/>
+    <col min="10" max="10" width="26.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:17">
+      <c r="B3" s="98" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3" s="61"/>
+      <c r="D3" s="61"/>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="62"/>
+      <c r="K3" s="99" t="s">
+        <v>142</v>
+      </c>
+      <c r="L3" s="61"/>
+      <c r="M3" s="61"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="61"/>
+      <c r="P3" s="61"/>
+      <c r="Q3" s="62"/>
+    </row>
+    <row r="4" spans="2:17">
+      <c r="B4" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>77</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="83" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="61"/>
+      <c r="H4" s="62"/>
+      <c r="K4" s="74" t="s">
+        <v>77</v>
+      </c>
+      <c r="L4" s="61"/>
+      <c r="M4" s="61"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="61"/>
+      <c r="P4" s="61"/>
+      <c r="Q4" s="62"/>
+    </row>
+    <row r="5" spans="2:17">
+      <c r="B5" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" s="41">
+        <v>1</v>
+      </c>
+      <c r="D5" s="39" t="s">
+        <v>115</v>
+      </c>
+      <c r="E5" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="F5" s="84">
+        <v>44811</v>
+      </c>
+      <c r="G5" s="61"/>
+      <c r="H5" s="62"/>
+      <c r="K5" s="79">
+        <v>1</v>
+      </c>
+      <c r="L5" s="61"/>
+      <c r="M5" s="61"/>
+      <c r="N5" s="61"/>
+      <c r="O5" s="61"/>
+      <c r="P5" s="61"/>
+      <c r="Q5" s="62"/>
+    </row>
+    <row r="6" spans="2:17">
+      <c r="B6" s="43" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6" s="41">
+        <v>2</v>
+      </c>
+      <c r="D6" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="E6" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="F6" s="84">
+        <v>44788</v>
+      </c>
+      <c r="G6" s="61"/>
+      <c r="H6" s="62"/>
+      <c r="K6" s="79">
+        <v>2</v>
+      </c>
+      <c r="L6" s="61"/>
+      <c r="M6" s="61"/>
+      <c r="N6" s="61"/>
+      <c r="O6" s="61"/>
+      <c r="P6" s="61"/>
+      <c r="Q6" s="62"/>
+    </row>
+    <row r="7" spans="2:17">
+      <c r="B7" s="45"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="79"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="61"/>
+      <c r="H7" s="62"/>
+      <c r="K7" s="79"/>
+      <c r="L7" s="61"/>
+      <c r="M7" s="61"/>
+      <c r="N7" s="61"/>
+      <c r="O7" s="61"/>
+      <c r="P7" s="61"/>
+      <c r="Q7" s="62"/>
+    </row>
+    <row r="11" spans="2:17">
+      <c r="G11" s="91" t="s">
+        <v>135</v>
+      </c>
+      <c r="H11" s="92"/>
+      <c r="I11" s="92"/>
+      <c r="J11" s="92"/>
+      <c r="K11" s="92"/>
+      <c r="L11" s="92"/>
+      <c r="M11" s="92"/>
+      <c r="N11" s="93"/>
+    </row>
+    <row r="12" spans="2:17">
+      <c r="G12" s="91" t="s">
+        <v>132</v>
+      </c>
+      <c r="H12" s="92"/>
+      <c r="I12" s="92"/>
+      <c r="J12" s="92"/>
+      <c r="K12" s="92"/>
+      <c r="L12" s="92"/>
+      <c r="M12" s="92"/>
+      <c r="N12" s="93"/>
+    </row>
+    <row r="13" spans="2:17">
+      <c r="G13" s="58" t="s">
+        <v>136</v>
+      </c>
+      <c r="H13" s="59" t="s">
+        <v>137</v>
+      </c>
+      <c r="I13" s="54" t="s">
+        <v>140</v>
+      </c>
+      <c r="J13" s="54" t="s">
+        <v>139</v>
+      </c>
+      <c r="K13" s="94" t="s">
+        <v>138</v>
+      </c>
+      <c r="L13" s="89"/>
+      <c r="M13" s="89"/>
+      <c r="N13" s="90"/>
+    </row>
+    <row r="14" spans="2:17">
+      <c r="G14" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="H14" s="41">
+        <v>1</v>
+      </c>
+      <c r="I14" s="39" t="s">
+        <v>115</v>
+      </c>
+      <c r="J14" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="K14" s="95">
+        <v>44811</v>
+      </c>
+      <c r="L14" s="96"/>
+      <c r="M14" s="96"/>
+      <c r="N14" s="97"/>
+    </row>
+    <row r="15" spans="2:17">
+      <c r="G15" s="43" t="s">
+        <v>117</v>
+      </c>
+      <c r="H15" s="41">
+        <v>2</v>
+      </c>
+      <c r="I15" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="J15" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="K15" s="95">
+        <v>44788</v>
+      </c>
+      <c r="L15" s="96"/>
+      <c r="M15" s="96"/>
+      <c r="N15" s="97"/>
+    </row>
+    <row r="16" spans="2:17">
+      <c r="G16" s="48"/>
+      <c r="H16" s="51"/>
+      <c r="I16" s="55"/>
+      <c r="J16" s="56"/>
+      <c r="K16" s="81"/>
+      <c r="L16" s="61"/>
+      <c r="M16" s="61"/>
+      <c r="N16" s="62"/>
+    </row>
+    <row r="17" spans="7:14">
+      <c r="G17" s="48"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="55"/>
+      <c r="J17" s="56"/>
+      <c r="K17" s="81"/>
+      <c r="L17" s="61"/>
+      <c r="M17" s="61"/>
+      <c r="N17" s="62"/>
+    </row>
+    <row r="18" spans="7:14">
+      <c r="G18" s="48"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="55"/>
+      <c r="J18" s="56"/>
+      <c r="K18" s="81"/>
+      <c r="L18" s="61"/>
+      <c r="M18" s="61"/>
+      <c r="N18" s="62"/>
+    </row>
+  </sheetData>
+  <mergeCells count="18">
+    <mergeCell ref="K3:Q3"/>
+    <mergeCell ref="K4:Q4"/>
+    <mergeCell ref="K5:Q5"/>
+    <mergeCell ref="K6:Q6"/>
+    <mergeCell ref="K7:Q7"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="K17:N17"/>
+    <mergeCell ref="K18:N18"/>
+    <mergeCell ref="G11:N11"/>
+    <mergeCell ref="G12:N12"/>
+    <mergeCell ref="K13:N13"/>
+    <mergeCell ref="K14:N14"/>
+    <mergeCell ref="K15:N15"/>
+    <mergeCell ref="K16:N16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>